<commit_message>
mise à jour du jdb
</commit_message>
<xml_diff>
--- a/Documentation/JDB.xlsx
+++ b/Documentation/JDB.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>écriture de la suite du dossier de projet</t>
+  </si>
+  <si>
+    <t>Suite du dossier de projet</t>
+  </si>
+  <si>
+    <t>Mise à jour des Uses cases</t>
   </si>
 </sst>
 </file>
@@ -616,7 +622,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,6 +1074,12 @@
       <c r="B25">
         <v>8</v>
       </c>
+      <c r="C25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="13">
+        <v>2</v>
+      </c>
       <c r="F25" s="1">
         <v>43179</v>
       </c>
@@ -1076,6 +1088,12 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="13">
+        <v>2</v>
+      </c>
       <c r="F26" s="1">
         <v>43180</v>
       </c>
@@ -1084,6 +1102,12 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="13">
+        <v>2</v>
+      </c>
       <c r="F27" s="1">
         <v>43181</v>
       </c>

</xml_diff>

<commit_message>
Implémentation du straightforward algorithm
J'ai ajouté le straightforward algorithm, et tout à l'air de fonctionner. Maintenant, il faut que je fasse des tests, et que j'éclairsisse un peu le code
</commit_message>
<xml_diff>
--- a/Documentation/JDB.xlsx
+++ b/Documentation/JDB.xlsx
@@ -311,7 +311,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -338,6 +337,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,10 +655,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
+      <c r="A2" s="28">
         <v>43132</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -674,8 +676,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
@@ -691,8 +693,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="34"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="33"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -708,17 +710,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>43133</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="16">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="14">
@@ -729,8 +731,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
@@ -746,8 +748,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
@@ -763,8 +765,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -780,10 +782,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>43137</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="34">
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -795,8 +797,8 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="36"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
@@ -812,8 +814,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="36"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
@@ -823,16 +825,16 @@
       <c r="E11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="14">
         <v>43146</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
@@ -840,10 +842,10 @@
         <v>1</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="1">
+      <c r="F12" s="14">
         <v>43147</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="15">
         <v>2</v>
       </c>
     </row>
@@ -869,10 +871,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+      <c r="A14" s="28">
         <v>43139</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="31">
         <v>8</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -890,8 +892,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="8" t="s">
         <v>7</v>
       </c>
@@ -907,8 +909,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="8" t="s">
         <v>18</v>
       </c>
@@ -924,8 +926,8 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="8" t="s">
         <v>19</v>
       </c>
@@ -941,8 +943,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="34"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="11" t="s">
         <v>20</v>
       </c>
@@ -961,7 +963,7 @@
       <c r="A19" s="27">
         <v>43140</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="37">
         <v>2</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -979,10 +981,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+      <c r="A20" s="28">
         <v>43144</v>
       </c>
-      <c r="B20" s="35">
+      <c r="B20" s="34">
         <v>5</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1000,8 +1002,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="36"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="8" t="s">
         <v>23</v>
       </c>
@@ -1017,8 +1019,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="36"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="8" t="s">
         <v>24</v>
       </c>
@@ -1034,8 +1036,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="7"/>
       <c r="D23" s="18"/>
       <c r="E23" s="4"/>
@@ -1050,7 +1052,7 @@
       <c r="A24" s="27">
         <v>43145</v>
       </c>
-      <c r="B24" s="28">
+      <c r="B24" s="37">
         <v>1</v>
       </c>
       <c r="C24" s="23" t="s">

</xml_diff>

<commit_message>
mise à jour du jdt
</commit_message>
<xml_diff>
--- a/Documentation/JDB.xlsx
+++ b/Documentation/JDB.xlsx
@@ -115,7 +115,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +125,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -311,36 +317,38 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +632,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:G12"/>
+      <selection activeCell="G15" sqref="F15:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,10 +663,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+      <c r="A2" s="29">
         <v>43132</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="32">
         <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -676,8 +684,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
@@ -693,8 +701,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -710,10 +718,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="29">
         <v>43133</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="32">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -731,8 +739,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
@@ -748,8 +756,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
@@ -765,8 +773,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="33"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
@@ -782,10 +790,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="29">
         <v>43137</v>
       </c>
-      <c r="B9" s="34">
+      <c r="B9" s="35">
         <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -797,8 +805,8 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
@@ -814,8 +822,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="6" t="s">
         <v>7</v>
       </c>
@@ -833,8 +841,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="36"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
@@ -863,18 +871,18 @@
         <v>1</v>
       </c>
       <c r="E13" s="25"/>
-      <c r="F13" s="1">
+      <c r="F13" s="14">
         <v>43158</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
+      <c r="A14" s="29">
         <v>43139</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="32">
         <v>8</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -884,16 +892,16 @@
         <v>3</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="1">
+      <c r="F14" s="14">
         <v>43159</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="8" t="s">
         <v>7</v>
       </c>
@@ -901,16 +909,16 @@
         <v>2</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="1">
+      <c r="F15" s="14">
         <v>43160</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="32"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="8" t="s">
         <v>18</v>
       </c>
@@ -918,16 +926,16 @@
         <v>2</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="1">
+      <c r="F16" s="14">
         <v>43161</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="32"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="8" t="s">
         <v>19</v>
       </c>
@@ -935,16 +943,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="1">
+      <c r="F17" s="14">
         <v>43165</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="11" t="s">
         <v>20</v>
       </c>
@@ -963,7 +971,7 @@
       <c r="A19" s="27">
         <v>43140</v>
       </c>
-      <c r="B19" s="37">
+      <c r="B19" s="28">
         <v>2</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -981,10 +989,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
+      <c r="A20" s="29">
         <v>43144</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="35">
         <v>5</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -994,16 +1002,16 @@
         <v>1</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="1">
+      <c r="F20" s="38">
         <v>43168</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="8" t="s">
         <v>23</v>
       </c>
@@ -1019,8 +1027,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="8" t="s">
         <v>24</v>
       </c>
@@ -1036,8 +1044,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="36"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="7"/>
       <c r="D23" s="18"/>
       <c r="E23" s="4"/>
@@ -1052,7 +1060,7 @@
       <c r="A24" s="27">
         <v>43145</v>
       </c>
-      <c r="B24" s="37">
+      <c r="B24" s="28">
         <v>1</v>
       </c>
       <c r="C24" s="23" t="s">

</xml_diff>